<commit_message>
XMLs vacíos, excels 2025 para pruebas
</commit_message>
<xml_diff>
--- a/resources/SistemasOrdenanzas.xlsx
+++ b/resources/SistemasOrdenanzas.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Documents\NetBeansProjects\vehiculos2025\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Nueva carpeta (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47706F83-D47D-4FD5-AB00-F6EDC0C6F1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A54839-59BF-409C-9B25-F6E80B776662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordenanza" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="20">
   <si>
     <t>TURISMO</t>
   </si>
@@ -79,6 +90,12 @@
   </si>
   <si>
     <t>BENAVIDES</t>
+  </si>
+  <si>
+    <t>ASTORGA</t>
+  </si>
+  <si>
+    <t>TRUCHAS</t>
   </si>
 </sst>
 </file>
@@ -134,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -174,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -280,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -430,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +962,966 @@
         <v>121.16</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>7.99</v>
+      </c>
+      <c r="F33">
+        <v>31.43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>11.99</v>
+      </c>
+      <c r="F34">
+        <v>87.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>15.99</v>
+      </c>
+      <c r="F35">
+        <v>193.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F36">
+        <v>251.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>9999</v>
+      </c>
+      <c r="F37">
+        <v>314.10000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>210.22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>21</v>
+      </c>
+      <c r="E41">
+        <v>50</v>
+      </c>
+      <c r="F41">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>51</v>
+      </c>
+      <c r="E42">
+        <v>9999</v>
+      </c>
+      <c r="F42">
+        <v>360.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>999</v>
+      </c>
+      <c r="F44">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
+      </c>
+      <c r="E45">
+        <v>2999</v>
+      </c>
+      <c r="F45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>3000</v>
+      </c>
+      <c r="E46">
+        <v>9999</v>
+      </c>
+      <c r="F46">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>10000</v>
+      </c>
+      <c r="E47">
+        <v>9999999</v>
+      </c>
+      <c r="F47">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>15.99</v>
+      </c>
+      <c r="F49">
+        <v>44.849999999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>16</v>
+      </c>
+      <c r="E50">
+        <v>25</v>
+      </c>
+      <c r="F50">
+        <v>70.349999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51">
+        <v>25.01</v>
+      </c>
+      <c r="E51">
+        <v>9999</v>
+      </c>
+      <c r="F51">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>751</v>
+      </c>
+      <c r="E53">
+        <v>999</v>
+      </c>
+      <c r="F53">
+        <v>44.849999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>1000</v>
+      </c>
+      <c r="E54">
+        <v>2999</v>
+      </c>
+      <c r="F54">
+        <v>70.349999999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>3000</v>
+      </c>
+      <c r="E55">
+        <v>9999999</v>
+      </c>
+      <c r="F55">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>49.99</v>
+      </c>
+      <c r="F57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>125</v>
+      </c>
+      <c r="F58">
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>125.01</v>
+      </c>
+      <c r="E59">
+        <v>250</v>
+      </c>
+      <c r="F59">
+        <v>22.71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>250.01</v>
+      </c>
+      <c r="E60">
+        <v>500</v>
+      </c>
+      <c r="F60">
+        <v>45.45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61">
+        <v>500.01</v>
+      </c>
+      <c r="E61">
+        <v>1000</v>
+      </c>
+      <c r="F61">
+        <v>87.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>1000.01</v>
+      </c>
+      <c r="E62">
+        <v>9999</v>
+      </c>
+      <c r="F62">
+        <v>181.74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>7.99</v>
+      </c>
+      <c r="F69">
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>11.99</v>
+      </c>
+      <c r="F70">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71">
+        <v>12</v>
+      </c>
+      <c r="E71">
+        <v>15.99</v>
+      </c>
+      <c r="F71">
+        <v>64.48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72">
+        <v>16</v>
+      </c>
+      <c r="E72">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F72">
+        <v>83.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="E73">
+        <v>9999</v>
+      </c>
+      <c r="F73">
+        <v>104.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>20</v>
+      </c>
+      <c r="F76">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77">
+        <v>21</v>
+      </c>
+      <c r="E77">
+        <v>50</v>
+      </c>
+      <c r="F77">
+        <v>99.68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78">
+        <v>51</v>
+      </c>
+      <c r="E78">
+        <v>9999</v>
+      </c>
+      <c r="F78">
+        <v>120.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>999</v>
+      </c>
+      <c r="F80">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81">
+        <v>1000</v>
+      </c>
+      <c r="E81">
+        <v>2999</v>
+      </c>
+      <c r="F81">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82">
+        <v>3000</v>
+      </c>
+      <c r="E82">
+        <v>9999</v>
+      </c>
+      <c r="F82">
+        <v>104.23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83">
+        <v>10000</v>
+      </c>
+      <c r="E83">
+        <v>9999999</v>
+      </c>
+      <c r="F83">
+        <v>135.93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>15.99</v>
+      </c>
+      <c r="F85">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86">
+        <v>16</v>
+      </c>
+      <c r="E86">
+        <v>25</v>
+      </c>
+      <c r="F86">
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>25.01</v>
+      </c>
+      <c r="E87">
+        <v>9999</v>
+      </c>
+      <c r="F87">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <v>751</v>
+      </c>
+      <c r="E89">
+        <v>999</v>
+      </c>
+      <c r="F89">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90">
+        <v>1000</v>
+      </c>
+      <c r="E90">
+        <v>2999</v>
+      </c>
+      <c r="F90">
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91">
+        <v>3000</v>
+      </c>
+      <c r="E91">
+        <v>9999999</v>
+      </c>
+      <c r="F91">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>49.99</v>
+      </c>
+      <c r="F93">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>125</v>
+      </c>
+      <c r="F94">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>19</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95">
+        <v>125.01</v>
+      </c>
+      <c r="E95">
+        <v>250</v>
+      </c>
+      <c r="F95">
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>19</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96">
+        <v>250.01</v>
+      </c>
+      <c r="E96">
+        <v>500</v>
+      </c>
+      <c r="F96">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97">
+        <v>500.01</v>
+      </c>
+      <c r="E97">
+        <v>1000</v>
+      </c>
+      <c r="F97">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B98" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>1000.01</v>
+      </c>
+      <c r="E98">
+        <v>9999</v>
+      </c>
+      <c r="F98">
+        <v>60.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Inicio generaReciboPDF y excels p5
</commit_message>
<xml_diff>
--- a/resources/SistemasOrdenanzas.xlsx
+++ b/resources/SistemasOrdenanzas.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Documents\NetBeansProjects\vehiculos2025\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Nueva carpeta (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47706F83-D47D-4FD5-AB00-F6EDC0C6F1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A54839-59BF-409C-9B25-F6E80B776662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordenanza" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="20">
   <si>
     <t>TURISMO</t>
   </si>
@@ -79,6 +90,12 @@
   </si>
   <si>
     <t>BENAVIDES</t>
+  </si>
+  <si>
+    <t>ASTORGA</t>
+  </si>
+  <si>
+    <t>TRUCHAS</t>
   </si>
 </sst>
 </file>
@@ -134,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -174,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -280,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -430,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +962,966 @@
         <v>121.16</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>7.99</v>
+      </c>
+      <c r="F33">
+        <v>31.43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>11.99</v>
+      </c>
+      <c r="F34">
+        <v>87.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>15.99</v>
+      </c>
+      <c r="F35">
+        <v>193.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F36">
+        <v>251.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>9999</v>
+      </c>
+      <c r="F37">
+        <v>314.10000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>210.22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>21</v>
+      </c>
+      <c r="E41">
+        <v>50</v>
+      </c>
+      <c r="F41">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>51</v>
+      </c>
+      <c r="E42">
+        <v>9999</v>
+      </c>
+      <c r="F42">
+        <v>360.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>999</v>
+      </c>
+      <c r="F44">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>1000</v>
+      </c>
+      <c r="E45">
+        <v>2999</v>
+      </c>
+      <c r="F45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>3000</v>
+      </c>
+      <c r="E46">
+        <v>9999</v>
+      </c>
+      <c r="F46">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>10000</v>
+      </c>
+      <c r="E47">
+        <v>9999999</v>
+      </c>
+      <c r="F47">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>15.99</v>
+      </c>
+      <c r="F49">
+        <v>44.849999999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>16</v>
+      </c>
+      <c r="E50">
+        <v>25</v>
+      </c>
+      <c r="F50">
+        <v>70.349999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51">
+        <v>25.01</v>
+      </c>
+      <c r="E51">
+        <v>9999</v>
+      </c>
+      <c r="F51">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>751</v>
+      </c>
+      <c r="E53">
+        <v>999</v>
+      </c>
+      <c r="F53">
+        <v>44.849999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>1000</v>
+      </c>
+      <c r="E54">
+        <v>2999</v>
+      </c>
+      <c r="F54">
+        <v>70.349999999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>3000</v>
+      </c>
+      <c r="E55">
+        <v>9999999</v>
+      </c>
+      <c r="F55">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>49.99</v>
+      </c>
+      <c r="F57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>125</v>
+      </c>
+      <c r="F58">
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>125.01</v>
+      </c>
+      <c r="E59">
+        <v>250</v>
+      </c>
+      <c r="F59">
+        <v>22.71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>250.01</v>
+      </c>
+      <c r="E60">
+        <v>500</v>
+      </c>
+      <c r="F60">
+        <v>45.45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61">
+        <v>500.01</v>
+      </c>
+      <c r="E61">
+        <v>1000</v>
+      </c>
+      <c r="F61">
+        <v>87.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>1000.01</v>
+      </c>
+      <c r="E62">
+        <v>9999</v>
+      </c>
+      <c r="F62">
+        <v>181.74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>7.99</v>
+      </c>
+      <c r="F69">
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>11.99</v>
+      </c>
+      <c r="F70">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71">
+        <v>12</v>
+      </c>
+      <c r="E71">
+        <v>15.99</v>
+      </c>
+      <c r="F71">
+        <v>64.48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72">
+        <v>16</v>
+      </c>
+      <c r="E72">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F72">
+        <v>83.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="E73">
+        <v>9999</v>
+      </c>
+      <c r="F73">
+        <v>104.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>20</v>
+      </c>
+      <c r="F76">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77">
+        <v>21</v>
+      </c>
+      <c r="E77">
+        <v>50</v>
+      </c>
+      <c r="F77">
+        <v>99.68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78">
+        <v>51</v>
+      </c>
+      <c r="E78">
+        <v>9999</v>
+      </c>
+      <c r="F78">
+        <v>120.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>999</v>
+      </c>
+      <c r="F80">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81">
+        <v>1000</v>
+      </c>
+      <c r="E81">
+        <v>2999</v>
+      </c>
+      <c r="F81">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82">
+        <v>3000</v>
+      </c>
+      <c r="E82">
+        <v>9999</v>
+      </c>
+      <c r="F82">
+        <v>104.23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83">
+        <v>10000</v>
+      </c>
+      <c r="E83">
+        <v>9999999</v>
+      </c>
+      <c r="F83">
+        <v>135.93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>15.99</v>
+      </c>
+      <c r="F85">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86">
+        <v>16</v>
+      </c>
+      <c r="E86">
+        <v>25</v>
+      </c>
+      <c r="F86">
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>25.01</v>
+      </c>
+      <c r="E87">
+        <v>9999</v>
+      </c>
+      <c r="F87">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <v>751</v>
+      </c>
+      <c r="E89">
+        <v>999</v>
+      </c>
+      <c r="F89">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90">
+        <v>1000</v>
+      </c>
+      <c r="E90">
+        <v>2999</v>
+      </c>
+      <c r="F90">
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91">
+        <v>3000</v>
+      </c>
+      <c r="E91">
+        <v>9999999</v>
+      </c>
+      <c r="F91">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>49.99</v>
+      </c>
+      <c r="F93">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>125</v>
+      </c>
+      <c r="F94">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>19</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95">
+        <v>125.01</v>
+      </c>
+      <c r="E95">
+        <v>250</v>
+      </c>
+      <c r="F95">
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>19</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96">
+        <v>250.01</v>
+      </c>
+      <c r="E96">
+        <v>500</v>
+      </c>
+      <c r="F96">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97">
+        <v>500.01</v>
+      </c>
+      <c r="E97">
+        <v>1000</v>
+      </c>
+      <c r="F97">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B98" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>1000.01</v>
+      </c>
+      <c r="E98">
+        <v>9999</v>
+      </c>
+      <c r="F98">
+        <v>60.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Imagen, librerías correctas, y archivos de resources vírgenes
</commit_message>
<xml_diff>
--- a/resources/SistemasOrdenanzas.xlsx
+++ b/resources/SistemasOrdenanzas.xlsx
@@ -5,38 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Nueva carpeta (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Desktop\practivcas 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A54839-59BF-409C-9B25-F6E80B776662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C174870D-BC36-4EA3-8804-5F86897DD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordenanza" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="21">
   <si>
     <t>TURISMO</t>
   </si>
@@ -97,6 +86,9 @@
   <si>
     <t>TRUCHAS</t>
   </si>
+  <si>
+    <t>VALVERDE</t>
+  </si>
 </sst>
 </file>
 
@@ -151,9 +143,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +183,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -297,7 +289,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,7 +431,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,6 +1914,486 @@
         <v>60.58</v>
       </c>
     </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>7.99</v>
+      </c>
+      <c r="F103">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104">
+        <v>8</v>
+      </c>
+      <c r="E104">
+        <v>11.99</v>
+      </c>
+      <c r="F104">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105">
+        <v>12</v>
+      </c>
+      <c r="E105">
+        <v>15.99</v>
+      </c>
+      <c r="F105">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106">
+        <v>16</v>
+      </c>
+      <c r="E106">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F106">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>13</v>
+      </c>
+      <c r="D107">
+        <v>20</v>
+      </c>
+      <c r="E107">
+        <v>9999</v>
+      </c>
+      <c r="F107">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>20</v>
+      </c>
+      <c r="F110">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111">
+        <v>21</v>
+      </c>
+      <c r="E111">
+        <v>50</v>
+      </c>
+      <c r="F111">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>20</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112">
+        <v>51</v>
+      </c>
+      <c r="E112">
+        <v>9999</v>
+      </c>
+      <c r="F112">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>999</v>
+      </c>
+      <c r="F114">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>20</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2</v>
+      </c>
+      <c r="C115" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115">
+        <v>1000</v>
+      </c>
+      <c r="E115">
+        <v>2999</v>
+      </c>
+      <c r="F115">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116">
+        <v>3000</v>
+      </c>
+      <c r="E116">
+        <v>9999</v>
+      </c>
+      <c r="F116">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2</v>
+      </c>
+      <c r="C117" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117">
+        <v>10000</v>
+      </c>
+      <c r="E117">
+        <v>9999999</v>
+      </c>
+      <c r="F117">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>20</v>
+      </c>
+      <c r="B119" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>15.99</v>
+      </c>
+      <c r="F119">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>20</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120">
+        <v>16</v>
+      </c>
+      <c r="E120">
+        <v>25</v>
+      </c>
+      <c r="F120">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>20</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121">
+        <v>25.01</v>
+      </c>
+      <c r="E121">
+        <v>9999</v>
+      </c>
+      <c r="F121">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" t="s">
+        <v>15</v>
+      </c>
+      <c r="D123">
+        <v>751</v>
+      </c>
+      <c r="E123">
+        <v>999</v>
+      </c>
+      <c r="F123">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" t="s">
+        <v>15</v>
+      </c>
+      <c r="D124">
+        <v>1000</v>
+      </c>
+      <c r="E124">
+        <v>2999</v>
+      </c>
+      <c r="F124">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>20</v>
+      </c>
+      <c r="B125" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125">
+        <v>3000</v>
+      </c>
+      <c r="E125">
+        <v>9999999</v>
+      </c>
+      <c r="F125">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>20</v>
+      </c>
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>49.99</v>
+      </c>
+      <c r="F127">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>125</v>
+      </c>
+      <c r="F128">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>20</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" t="s">
+        <v>16</v>
+      </c>
+      <c r="D129">
+        <v>125.01</v>
+      </c>
+      <c r="E129">
+        <v>250</v>
+      </c>
+      <c r="F129">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>20</v>
+      </c>
+      <c r="B130" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130">
+        <v>250.01</v>
+      </c>
+      <c r="E130">
+        <v>500</v>
+      </c>
+      <c r="F130">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>20</v>
+      </c>
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131">
+        <v>500.01</v>
+      </c>
+      <c r="E131">
+        <v>1000</v>
+      </c>
+      <c r="F131">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>20</v>
+      </c>
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132" t="s">
+        <v>16</v>
+      </c>
+      <c r="D132">
+        <v>1000.01</v>
+      </c>
+      <c r="E132">
+        <v>9999</v>
+      </c>
+      <c r="F132">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>